<commit_message>
Listo para productivo, correccion ruta planilla giros
</commit_message>
<xml_diff>
--- a/ServicesLayer/FirstRun/Data/Config.xlsx
+++ b/ServicesLayer/FirstRun/Data/Config.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -359,22 +359,25 @@
     <t>PlantillaGiroArchivo</t>
   </si>
   <si>
+    <t>PathHistoricoGiros</t>
+  </si>
+  <si>
+    <t>FacturasTEEX</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\TEEX\Pendientes RC</t>
+  </si>
+  <si>
+    <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\AGEX\Planillas giros\</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Planillas giros</t>
+  </si>
+  <si>
+    <t>jairo.andres@fouriering.com</t>
+  </si>
+  <si>
     <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Historico Giros</t>
-  </si>
-  <si>
-    <t>PathHistoricoGiros</t>
-  </si>
-  <si>
-    <t>yeraldin.cano@fouriering.com</t>
-  </si>
-  <si>
-    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Planillas giros\</t>
-  </si>
-  <si>
-    <t>FacturasTEEX</t>
-  </si>
-  <si>
-    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\TEEX\Pendientes RC</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1145,10 +1148,10 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>75</v>
@@ -1159,16 +1162,16 @@
         <v>109</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C11" s="18"/>
     </row>
@@ -1265,7 +1268,7 @@
         <v>98</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>99</v>
@@ -2275,14 +2278,11 @@
     <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataConsolidate/>
-  <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Desplegable!$B$2:$C$2</xm:f>
@@ -2293,7 +2293,7 @@
           <x14:formula1>
             <xm:f>Desplegable!$B$3:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B9 B11</xm:sqref>
+          <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2313,6 +2313,12 @@
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Desplegable!$B$7:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2321,15 +2327,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.5546875" customWidth="1"/>
     <col min="3" max="3" width="74.88671875" customWidth="1"/>
   </cols>
@@ -2358,10 +2364,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>70</v>
@@ -2398,6 +2404,17 @@
       </c>
       <c r="C6" s="18" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 1.1.0 para subir a productivo
</commit_message>
<xml_diff>
--- a/ServicesLayer/FirstRun/Data/Config.xlsx
+++ b/ServicesLayer/FirstRun/Data/Config.xlsx
@@ -371,13 +371,13 @@
     <t>O:\DISSEN\INSUMOS ROBOT RECAUDOS LEONISA\AGEX\Planillas giros\</t>
   </si>
   <si>
+    <t>jairo.andres@fouriering.com</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Historico Giros</t>
+  </si>
+  <si>
     <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Planillas giros</t>
-  </si>
-  <si>
-    <t>jairo.andres@fouriering.com</t>
-  </si>
-  <si>
-    <t>C:\Users\ROBTIRELEO\Documents\Recaudos\AGEX\Historico Giros</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1162,7 +1162,7 @@
         <v>109</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C10" s="18"/>
     </row>
@@ -1171,7 +1171,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="18"/>
     </row>
@@ -1268,7 +1268,7 @@
         <v>98</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>99</v>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2411,7 +2411,7 @@
         <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>113</v>

</xml_diff>